<commit_message>
refactor layers and return standart metrics MSE&MAE
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Без помех" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Фильтр нижних частот</t>
   </si>
@@ -27,16 +27,40 @@
   <si>
     <t>Нейросетевой фильтр</t>
   </si>
+  <si>
+    <t>, 0.15925, 0.02789, -1.58305, 13.89881</t>
+  </si>
+  <si>
+    <t>, 0.20221, 0.03076, -1.58451, 14.61147</t>
+  </si>
+  <si>
+    <t>, 0.23189, 0.03403, -1.58791, 16.03721</t>
+  </si>
+  <si>
+    <t>, 0.20123, 0.03524, -1.58969, 16.75113</t>
+  </si>
+  <si>
+    <t>, 0.20598, 0.03624, -1.59348, 18.18004</t>
+  </si>
+  <si>
+    <t>, 0.21760, 0.03756, -1.59554, 18.89430</t>
+  </si>
+  <si>
+    <t>, 0.26894, 0.04017, -1.59750, 19.60875</t>
+  </si>
+  <si>
+    <t>, 0.21590, 0.04001, -1.59951, 20.32340</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="180" formatCode="0.0000000"/>
-    <numFmt numFmtId="184" formatCode="0.00000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +93,15 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6897BB"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -209,7 +242,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFill="1" applyBorder="1"/>
@@ -221,6 +254,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -230,8 +265,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Вывод" xfId="2" builtinId="21"/>
@@ -539,13 +578,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
@@ -557,8 +596,8 @@
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:9">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
@@ -583,8 +622,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
+    <row r="2" spans="2:9">
+      <c r="B2" s="14"/>
       <c r="C2" s="4">
         <v>5.3100116987414602E-4</v>
       </c>
@@ -607,8 +646,8 @@
         <v>6.55419108403214E-4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
+    <row r="3" spans="2:9">
+      <c r="B3" s="14"/>
       <c r="C3" s="4">
         <v>5.5724726974416296E-4</v>
       </c>
@@ -631,8 +670,8 @@
         <v>8.4494374572411995E-4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B4" s="14"/>
       <c r="C4" s="7">
         <f>(C2-MIN($C$2:$I$2))/MIN($C$2:$I$2) * 100</f>
         <v>8.6852407028907166</v>
@@ -662,8 +701,8 @@
         <v>34.151085909962845</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B5" s="15"/>
       <c r="C5" s="7">
         <f>(C3-MIN($C$3:$I$3))/MIN($C$3:$I$3) * 100</f>
         <v>6.2505526954919715</v>
@@ -693,8 +732,8 @@
         <v>61.105751170398371</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:9">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1">
@@ -719,8 +758,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+    <row r="7" spans="2:9">
+      <c r="B7" s="14"/>
       <c r="C7" s="4">
         <v>4.6033177016613098E-4</v>
       </c>
@@ -743,8 +782,8 @@
         <v>4.0204613321015502E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+    <row r="8" spans="2:9">
+      <c r="B8" s="14"/>
       <c r="C8" s="4">
         <v>5.0966284511161104E-4</v>
       </c>
@@ -767,8 +806,8 @@
         <v>4.0200146616198702E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+    <row r="9" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B9" s="14"/>
       <c r="C9" s="7">
         <f>(C7-MIN($C7:$I7))/MIN($C7:$I7) * 100</f>
         <v>14.497250972317961</v>
@@ -798,8 +837,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+    <row r="10" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B10" s="15"/>
       <c r="C10" s="7">
         <f>(C8-MIN($C8:$I8))/MIN($C8:$I8) * 100</f>
         <v>26.781339873581882</v>
@@ -829,8 +868,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="2:9">
+      <c r="B11" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1">
@@ -855,8 +894,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+    <row r="12" spans="2:9">
+      <c r="B12" s="14"/>
       <c r="C12" s="4">
         <v>3.7860568027613502E-4</v>
       </c>
@@ -879,8 +918,8 @@
         <v>3.0517433972899799E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+    <row r="13" spans="2:9">
+      <c r="B13" s="14"/>
       <c r="C13" s="4">
         <v>3.6041840679270297E-4</v>
       </c>
@@ -903,8 +942,8 @@
         <v>3.0394042171795298E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B14" s="14"/>
       <c r="C14" s="7">
         <f>(C12-MIN($C12:$I12))/MIN($C12:$I12) * 100</f>
         <v>24.062095329622338</v>
@@ -934,8 +973,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B15" s="15"/>
       <c r="C15" s="7">
         <f>(C13-MIN($C13:$I13))/MIN($C13:$I13) * 100</f>
         <v>18.581926272103342</v>
@@ -965,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="C16" s="10">
         <v>1</v>
       </c>
@@ -988,15 +1027,127 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="11">
         <v>1.4660000000000001E-4</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>2.4490999999999999E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="D26">
+        <v>13.898809999999999</v>
+      </c>
+      <c r="E26" s="16">
+        <f>D26/60</f>
+        <v>0.23164683333333333</v>
+      </c>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="D27">
+        <v>14.611470000000001</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" ref="E27:E33" si="6">D27/60</f>
+        <v>0.2435245</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="D28">
+        <v>16.037210000000002</v>
+      </c>
+      <c r="E28" s="16">
+        <f t="shared" si="6"/>
+        <v>0.26728683333333336</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="D29">
+        <v>16.75113</v>
+      </c>
+      <c r="E29" s="16">
+        <f t="shared" si="6"/>
+        <v>0.27918549999999998</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="D30">
+        <v>18.180040000000002</v>
+      </c>
+      <c r="E30" s="16">
+        <f t="shared" si="6"/>
+        <v>0.3030006666666667</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="I30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="D31">
+        <v>18.894300000000001</v>
+      </c>
+      <c r="E31" s="16">
+        <f t="shared" si="6"/>
+        <v>0.31490500000000005</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="I31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="D32">
+        <v>19.608750000000001</v>
+      </c>
+      <c r="E32" s="16">
+        <f t="shared" si="6"/>
+        <v>0.32681250000000001</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9">
+      <c r="D33">
+        <v>20.323399999999999</v>
+      </c>
+      <c r="E33" s="16">
+        <f t="shared" si="6"/>
+        <v>0.33872333333333332</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9">
+      <c r="E34" s="16"/>
+      <c r="I34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9">
+      <c r="I35" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1006,6 +1157,6 @@
     <mergeCell ref="B11:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>